<commit_message>
Added support for csv files
</commit_message>
<xml_diff>
--- a/Ne_Lines_fit_loop.xlsx
+++ b/Ne_Lines_fit_loop.xlsx
@@ -615,25 +615,25 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1453.430928757286</v>
+        <v>1453.432283074141</v>
       </c>
       <c r="D2">
-        <v>0.0049</v>
+        <v>0.008319999999999999</v>
       </c>
       <c r="E2">
-        <v>1122.852586669516</v>
+        <v>1122.853301962157</v>
       </c>
       <c r="G2">
-        <v>330.5783420877694</v>
+        <v>330.5789811119839</v>
       </c>
       <c r="H2">
-        <v>0.9996953578775506</v>
+        <v>0.9996934254209296</v>
       </c>
       <c r="K2">
-        <v>66.47359396050969</v>
+        <v>117.6856218310954</v>
       </c>
       <c r="L2">
-        <v>10.72891505502725</v>
+        <v>8.863946411354874</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -644,25 +644,25 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1453.399337040959</v>
+        <v>1453.400732521733</v>
       </c>
       <c r="D3">
-        <v>0.00594</v>
+        <v>0.00944</v>
       </c>
       <c r="E3">
-        <v>1122.833578389602</v>
+        <v>1122.834056781906</v>
       </c>
       <c r="G3">
-        <v>330.5657586513571</v>
+        <v>330.5666757398276</v>
       </c>
       <c r="H3">
-        <v>0.9997334126446834</v>
+        <v>0.9997306390923154</v>
       </c>
       <c r="K3">
-        <v>88.12907440247028</v>
+        <v>147.5812644181681</v>
       </c>
       <c r="L3">
-        <v>10.03370699827812</v>
+        <v>8.025353646303792</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -673,25 +673,25 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1453.404072980472</v>
+        <v>1453.40541272591</v>
       </c>
       <c r="D4">
-        <v>0.00551</v>
+        <v>0.00911</v>
       </c>
       <c r="E4">
-        <v>1122.826791340547</v>
+        <v>1122.827264394749</v>
       </c>
       <c r="G4">
-        <v>330.5772816399253</v>
+        <v>330.5781483311612</v>
       </c>
       <c r="H4">
-        <v>0.9996985647669707</v>
+        <v>0.999695943813381</v>
       </c>
       <c r="K4">
-        <v>83.10593463346997</v>
+        <v>143.1983993045522</v>
       </c>
       <c r="L4">
-        <v>10.29012055816428</v>
+        <v>8.260495712171181</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -702,25 +702,25 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1453.403444031489</v>
+        <v>1453.404806924505</v>
       </c>
       <c r="D5">
-        <v>0.00594</v>
+        <v>0.00962</v>
       </c>
       <c r="E5">
-        <v>1122.820609587561</v>
+        <v>1122.82104104081</v>
       </c>
       <c r="G5">
-        <v>330.5828344439276</v>
+        <v>330.5837658836956</v>
       </c>
       <c r="H5">
-        <v>0.9996817728176827</v>
+        <v>0.9996789561537849</v>
       </c>
       <c r="K5">
-        <v>90.68164262037845</v>
+        <v>153.1442351912575</v>
       </c>
       <c r="L5">
-        <v>10.18303870929214</v>
+        <v>8.447985797372823</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -731,25 +731,25 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>1453.40064459076</v>
+        <v>1453.40195878175</v>
       </c>
       <c r="D6">
-        <v>0.00572</v>
+        <v>0.0095</v>
       </c>
       <c r="E6">
-        <v>1122.826020758853</v>
+        <v>1122.826475307605</v>
       </c>
       <c r="G6">
-        <v>330.5746238319075</v>
+        <v>330.5754834741451</v>
       </c>
       <c r="H6">
-        <v>0.9997066023072697</v>
+        <v>0.9997040026286379</v>
       </c>
       <c r="K6">
-        <v>87.41812246454055</v>
+        <v>150.3767867722999</v>
       </c>
       <c r="L6">
-        <v>10.68297557665008</v>
+        <v>8.413107421307732</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -760,25 +760,25 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>1453.400816599938</v>
+        <v>1453.402136199878</v>
       </c>
       <c r="D7">
-        <v>0.00576</v>
+        <v>0.009429999999999999</v>
       </c>
       <c r="E7">
-        <v>1122.766220080753</v>
+        <v>1122.766481401195</v>
       </c>
       <c r="G7">
-        <v>330.6345965191854</v>
+        <v>330.6356547986832</v>
       </c>
       <c r="H7">
-        <v>0.9995252689197144</v>
+        <v>0.9995220696969921</v>
       </c>
       <c r="K7">
-        <v>88.40010891510407</v>
+        <v>151.5969586228231</v>
       </c>
       <c r="L7">
-        <v>19.52099508474029</v>
+        <v>18.21686615047521</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -789,25 +789,25 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1453.39795943578</v>
+        <v>1453.399165406868</v>
       </c>
       <c r="D8">
-        <v>0.00521</v>
+        <v>0.00893</v>
       </c>
       <c r="E8">
-        <v>1122.833013933787</v>
+        <v>1122.833645455433</v>
       </c>
       <c r="G8">
-        <v>330.564945501993</v>
+        <v>330.5655199514347</v>
       </c>
       <c r="H8">
-        <v>0.9997358718666907</v>
+        <v>0.9997341345478271</v>
       </c>
       <c r="K8">
-        <v>78.57782077935776</v>
+        <v>140.5239106359868</v>
       </c>
       <c r="L8">
-        <v>9.378425399639099</v>
+        <v>7.530874046844596</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -818,25 +818,25 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>1453.39591111102</v>
+        <v>1453.397186443319</v>
       </c>
       <c r="D9">
-        <v>0.00544</v>
+        <v>0.00928</v>
       </c>
       <c r="E9">
-        <v>1122.838714857813</v>
+        <v>1122.839245182774</v>
       </c>
       <c r="G9">
-        <v>330.5571962532069</v>
+        <v>330.557941260545</v>
       </c>
       <c r="H9">
-        <v>0.9997593086639507</v>
+        <v>0.9997570554189721</v>
       </c>
       <c r="K9">
-        <v>84.14039363597203</v>
+        <v>150.5045703751539</v>
       </c>
       <c r="L9">
-        <v>9.733345258786201</v>
+        <v>7.184123259564132</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -847,25 +847,25 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>1453.393581428515</v>
+        <v>1453.394864163264</v>
       </c>
       <c r="D10">
-        <v>0.0057</v>
+        <v>0.00942</v>
       </c>
       <c r="E10">
-        <v>1122.820388098725</v>
+        <v>1122.821014551276</v>
       </c>
       <c r="G10">
-        <v>330.5731933297905</v>
+        <v>330.573849611988</v>
       </c>
       <c r="H10">
-        <v>0.9997109283761703</v>
+        <v>0.9997089436684091</v>
       </c>
       <c r="K10">
-        <v>89.69193761304587</v>
+        <v>154.8909581475111</v>
       </c>
       <c r="L10">
-        <v>10.30636502335662</v>
+        <v>7.895164613244239</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -876,25 +876,25 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>1453.393897272939</v>
+        <v>1453.395154401835</v>
       </c>
       <c r="D11">
-        <v>0.00567</v>
+        <v>0.00944</v>
       </c>
       <c r="E11">
-        <v>1122.835069272484</v>
+        <v>1122.835594824286</v>
       </c>
       <c r="G11">
-        <v>330.5588280004549</v>
+        <v>330.559559577549</v>
       </c>
       <c r="H11">
-        <v>0.999754373522722</v>
+        <v>0.9997521609187354</v>
       </c>
       <c r="K11">
-        <v>96.65823922120465</v>
+        <v>169.2964505793923</v>
       </c>
       <c r="L11">
-        <v>11.04819842471952</v>
+        <v>8.45128899537715</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -905,25 +905,25 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>1453.39716596795</v>
+        <v>1453.398401807514</v>
       </c>
       <c r="D12">
-        <v>0.00542</v>
+        <v>0.00908</v>
       </c>
       <c r="E12">
-        <v>1122.812036282069</v>
+        <v>1122.8124526751</v>
       </c>
       <c r="G12">
-        <v>330.5851296858807</v>
+        <v>330.5859491324138</v>
       </c>
       <c r="H12">
-        <v>0.9996748320591951</v>
+        <v>0.9996723540952117</v>
       </c>
       <c r="K12">
-        <v>73.5319332504702</v>
+        <v>128.6720716666637</v>
       </c>
       <c r="L12">
-        <v>9.428110658003568</v>
+        <v>7.641159579844889</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -934,25 +934,25 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>1453.422933935878</v>
+        <v>1453.424195688298</v>
       </c>
       <c r="D13">
-        <v>0.00464</v>
+        <v>0.00804</v>
       </c>
       <c r="E13">
-        <v>1122.858576769864</v>
+        <v>1122.859250944766</v>
       </c>
       <c r="G13">
-        <v>330.5643571660141</v>
+        <v>330.5649447435328</v>
       </c>
       <c r="H13">
-        <v>0.9997376511891433</v>
+        <v>0.9997358741605208</v>
       </c>
       <c r="K13">
-        <v>61.8737293325974</v>
+        <v>112.323333971182</v>
       </c>
       <c r="L13">
-        <v>9.153840345711071</v>
+        <v>6.912681441734127</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -963,25 +963,25 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>1453.397086948706</v>
+        <v>1453.398240556306</v>
       </c>
       <c r="D14">
-        <v>0.00565</v>
+        <v>0.0094</v>
       </c>
       <c r="E14">
-        <v>1122.818685924849</v>
+        <v>1122.819188389163</v>
       </c>
       <c r="G14">
-        <v>330.5784010238569</v>
+        <v>330.5790521671424</v>
       </c>
       <c r="H14">
-        <v>0.999695179650138</v>
+        <v>0.9996932105453218</v>
       </c>
       <c r="K14">
-        <v>76.18193863641079</v>
+        <v>131.2692489870473</v>
       </c>
       <c r="L14">
-        <v>10.26035271765904</v>
+        <v>8.223554461424461</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -992,25 +992,25 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>1453.398852393296</v>
+        <v>1453.400125082121</v>
       </c>
       <c r="D15">
-        <v>0.00559</v>
+        <v>0.009350000000000001</v>
       </c>
       <c r="E15">
-        <v>1122.834490519636</v>
+        <v>1122.835040469734</v>
       </c>
       <c r="G15">
-        <v>330.5643618736606</v>
+        <v>330.5650846123874</v>
       </c>
       <c r="H15">
-        <v>0.9997376369516394</v>
+        <v>0.999735451151806</v>
       </c>
       <c r="K15">
-        <v>74.65328595222174</v>
+        <v>129.670495450618</v>
       </c>
       <c r="L15">
-        <v>9.670902586163605</v>
+        <v>7.599776936852114</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1021,25 +1021,25 @@
         <v>25</v>
       </c>
       <c r="C16">
-        <v>1453.398750271513</v>
+        <v>1453.399945926383</v>
       </c>
       <c r="D16">
-        <v>0.00535</v>
+        <v>0.0091</v>
       </c>
       <c r="E16">
-        <v>1122.827744904191</v>
+        <v>1122.828259515415</v>
       </c>
       <c r="G16">
-        <v>330.5710053673222</v>
+        <v>330.5716864109677</v>
       </c>
       <c r="H16">
-        <v>0.9997175451996511</v>
+        <v>0.9997154855819965</v>
       </c>
       <c r="K16">
-        <v>71.76814906664758</v>
+        <v>126.3246157780197</v>
       </c>
       <c r="L16">
-        <v>9.699092895245453</v>
+        <v>7.972181873114105</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1050,25 +1050,25 @@
         <v>26</v>
       </c>
       <c r="C17">
-        <v>1453.397496228781</v>
+        <v>1453.398681945109</v>
       </c>
       <c r="D17">
-        <v>0.00547</v>
+        <v>0.009129999999999999</v>
       </c>
       <c r="E17">
-        <v>1122.771719052272</v>
+        <v>1122.771635952594</v>
       </c>
       <c r="G17">
-        <v>330.6257771765086</v>
+        <v>330.6270459925151</v>
       </c>
       <c r="H17">
-        <v>0.9995519309541632</v>
+        <v>0.9995480950686699</v>
       </c>
       <c r="K17">
-        <v>72.47065487019938</v>
+        <v>126.7752418540055</v>
       </c>
       <c r="L17">
-        <v>14.62216249328626</v>
+        <v>12.69288214398246</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1079,25 +1079,25 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>1453.398308318256</v>
+        <v>1453.399421068427</v>
       </c>
       <c r="D18">
-        <v>0.00497</v>
+        <v>0.00873</v>
       </c>
       <c r="E18">
-        <v>1122.822219623588</v>
+        <v>1122.822733746294</v>
       </c>
       <c r="G18">
-        <v>330.5760886946684</v>
+        <v>330.5766873221326</v>
       </c>
       <c r="H18">
-        <v>0.9997021723650455</v>
+        <v>0.9997003620462928</v>
       </c>
       <c r="K18">
-        <v>63.82698941421673</v>
+        <v>116.6744707638202</v>
       </c>
       <c r="L18">
-        <v>9.068662312192298</v>
+        <v>6.737258119396641</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1108,25 +1108,25 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>1453.399441686641</v>
+        <v>1453.400556965505</v>
       </c>
       <c r="D19">
-        <v>0.00523</v>
+        <v>0.0089</v>
       </c>
       <c r="E19">
-        <v>1122.831413902102</v>
+        <v>1122.831930066674</v>
       </c>
       <c r="G19">
-        <v>330.5680277845383</v>
+        <v>330.5686268988309</v>
       </c>
       <c r="H19">
-        <v>0.9997265501290487</v>
+        <v>0.9997247382497109</v>
       </c>
       <c r="K19">
-        <v>65.11421135230378</v>
+        <v>115.4532623955159</v>
       </c>
       <c r="L19">
-        <v>9.711079278557726</v>
+        <v>7.607799137631153</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1137,25 +1137,25 @@
         <v>29</v>
       </c>
       <c r="C20">
-        <v>1453.400536469242</v>
+        <v>1453.401688060507</v>
       </c>
       <c r="D20">
-        <v>0.00529</v>
+        <v>0.009010000000000001</v>
       </c>
       <c r="E20">
-        <v>1122.829074580165</v>
+        <v>1122.829730543114</v>
       </c>
       <c r="G20">
-        <v>330.571461889077</v>
+        <v>330.5719575173932</v>
       </c>
       <c r="H20">
-        <v>0.9997161645819612</v>
+        <v>0.9997146657021316</v>
       </c>
       <c r="K20">
-        <v>68.44599474075602</v>
+        <v>120.863561511025</v>
       </c>
       <c r="L20">
-        <v>10.2943035442363</v>
+        <v>8.213614607104105</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1166,25 +1166,25 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>1453.403667568319</v>
+        <v>1453.404890429623</v>
       </c>
       <c r="D21">
-        <v>0.00546</v>
+        <v>0.009129999999999999</v>
       </c>
       <c r="E21">
-        <v>1122.832928819716</v>
+        <v>1122.833518272695</v>
       </c>
       <c r="G21">
-        <v>330.5707387486032</v>
+        <v>330.5713721569275</v>
       </c>
       <c r="H21">
-        <v>0.9997183515124309</v>
+        <v>0.9997164359505306</v>
       </c>
       <c r="K21">
-        <v>75.2717669288414</v>
+        <v>129.6797072271276</v>
       </c>
       <c r="L21">
-        <v>9.432447899516717</v>
+        <v>7.094826441163498</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1195,25 +1195,25 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>1453.410467691493</v>
+        <v>1453.411629316387</v>
       </c>
       <c r="D22">
-        <v>0.0052</v>
+        <v>0.009010000000000001</v>
       </c>
       <c r="E22">
-        <v>1122.835561349134</v>
+        <v>1122.836259909168</v>
       </c>
       <c r="G22">
-        <v>330.5749063423589</v>
+        <v>330.5753694072189</v>
       </c>
       <c r="H22">
-        <v>0.9997057479545707</v>
+        <v>0.9997043475822348</v>
       </c>
       <c r="K22">
-        <v>71.3136824871081</v>
+        <v>129.4940500368449</v>
       </c>
       <c r="L22">
-        <v>9.279714349272911</v>
+        <v>6.992383093937766</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1224,25 +1224,25 @@
         <v>32</v>
       </c>
       <c r="C23">
-        <v>1453.412011516353</v>
+        <v>1453.41320070295</v>
       </c>
       <c r="D23">
-        <v>0.00511</v>
+        <v>0.00885</v>
       </c>
       <c r="E23">
-        <v>1122.830729836016</v>
+        <v>1122.831242471528</v>
       </c>
       <c r="G23">
-        <v>330.5812816803364</v>
+        <v>330.581958231422</v>
       </c>
       <c r="H23">
-        <v>0.9996864683934629</v>
+        <v>0.9996844224894179</v>
       </c>
       <c r="K23">
-        <v>68.55567949511916</v>
+        <v>124.3867670370455</v>
       </c>
       <c r="L23">
-        <v>9.487221177163136</v>
+        <v>7.359521055484505</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1253,25 +1253,25 @@
         <v>33</v>
       </c>
       <c r="C24">
-        <v>1453.423426971579</v>
+        <v>1453.424793104965</v>
       </c>
       <c r="D24">
-        <v>0.0051</v>
+        <v>0.00848</v>
       </c>
       <c r="E24">
-        <v>1122.856649440743</v>
+        <v>1122.857260364136</v>
       </c>
       <c r="G24">
-        <v>330.5667775308357</v>
+        <v>330.5675327408294</v>
       </c>
       <c r="H24">
-        <v>0.999730331246529</v>
+        <v>0.9997280472765006</v>
       </c>
       <c r="K24">
-        <v>73.58247023865601</v>
+        <v>127.7318205134149</v>
       </c>
       <c r="L24">
-        <v>9.335960622359305</v>
+        <v>7.158906503567191</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1282,25 +1282,25 @@
         <v>34</v>
       </c>
       <c r="C25">
-        <v>1453.406394667976</v>
+        <v>1453.407509383097</v>
       </c>
       <c r="D25">
-        <v>0.00524</v>
+        <v>0.00902</v>
       </c>
       <c r="E25">
-        <v>1122.834612914048</v>
+        <v>1122.835175886551</v>
       </c>
       <c r="G25">
-        <v>330.5717817539282</v>
+        <v>330.5723334965458</v>
       </c>
       <c r="H25">
-        <v>0.9997151972457278</v>
+        <v>0.999713528668464</v>
       </c>
       <c r="K25">
-        <v>68.63088754947123</v>
+        <v>122.2360394474033</v>
       </c>
       <c r="L25">
-        <v>9.429592963745268</v>
+        <v>6.9572238162545</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1311,25 +1311,25 @@
         <v>35</v>
       </c>
       <c r="C26">
-        <v>1453.409207033651</v>
+        <v>1453.410338411024</v>
       </c>
       <c r="D26">
-        <v>0.00498</v>
+        <v>0.008750000000000001</v>
       </c>
       <c r="E26">
-        <v>1122.821369497712</v>
+        <v>1122.821830885331</v>
       </c>
       <c r="G26">
-        <v>330.5878375359387</v>
+        <v>330.5885075256936</v>
       </c>
       <c r="H26">
-        <v>0.999666643707282</v>
+        <v>0.9996646177251491</v>
       </c>
       <c r="K26">
-        <v>68.67747688807859</v>
+        <v>126.1463953838188</v>
       </c>
       <c r="L26">
-        <v>9.445781447243128</v>
+        <v>7.522866683842173</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1340,25 +1340,25 @@
         <v>36</v>
       </c>
       <c r="C27">
-        <v>1453.406665452365</v>
+        <v>1453.407836653391</v>
       </c>
       <c r="D27">
-        <v>0.0051</v>
+        <v>0.00889</v>
       </c>
       <c r="E27">
-        <v>1122.821460259318</v>
+        <v>1122.821828922799</v>
       </c>
       <c r="G27">
-        <v>330.5852051930474</v>
+        <v>330.586007730592</v>
       </c>
       <c r="H27">
-        <v>0.9996746037289099</v>
+        <v>0.9996721768978187</v>
       </c>
       <c r="K27">
-        <v>69.75889347519298</v>
+        <v>126.56854346632</v>
       </c>
       <c r="L27">
-        <v>9.112394873821977</v>
+        <v>6.873357966798632</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1369,25 +1369,25 @@
         <v>37</v>
       </c>
       <c r="C28">
-        <v>1453.404040149883</v>
+        <v>1453.405174985635</v>
       </c>
       <c r="D28">
-        <v>0.00536</v>
+        <v>0.009129999999999999</v>
       </c>
       <c r="E28">
-        <v>1122.828791011425</v>
+        <v>1122.829223443528</v>
       </c>
       <c r="G28">
-        <v>330.5752491384583</v>
+        <v>330.5759515421071</v>
       </c>
       <c r="H28">
-        <v>0.9997047112912638</v>
+        <v>0.9997025871311921</v>
       </c>
       <c r="K28">
-        <v>72.29371485845175</v>
+        <v>128.1680591663873</v>
       </c>
       <c r="L28">
-        <v>9.487282418338104</v>
+        <v>7.576694801717728</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1398,25 +1398,25 @@
         <v>38</v>
       </c>
       <c r="C29">
-        <v>1453.404362054351</v>
+        <v>1453.405578464682</v>
       </c>
       <c r="D29">
-        <v>0.00521</v>
+        <v>0.008840000000000001</v>
       </c>
       <c r="E29">
-        <v>1122.834504620139</v>
+        <v>1122.834969901038</v>
       </c>
       <c r="G29">
-        <v>330.5698574342125</v>
+        <v>330.5706085636439</v>
       </c>
       <c r="H29">
-        <v>0.9997210168073754</v>
+        <v>0.9997187452204301</v>
       </c>
       <c r="K29">
-        <v>70.32999071906077</v>
+        <v>124.7411210763951</v>
       </c>
       <c r="L29">
-        <v>9.661968638491263</v>
+        <v>7.613545417800535</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1427,25 +1427,25 @@
         <v>39</v>
       </c>
       <c r="C30">
-        <v>1453.404855990041</v>
+        <v>1453.405978741109</v>
       </c>
       <c r="D30">
-        <v>0.0052</v>
+        <v>0.008920000000000001</v>
       </c>
       <c r="E30">
-        <v>1122.823799730068</v>
+        <v>1122.824324886349</v>
       </c>
       <c r="G30">
-        <v>330.5810562599734</v>
+        <v>330.5816538547601</v>
       </c>
       <c r="H30">
-        <v>0.9996871500710192</v>
+        <v>0.9996853429295087</v>
       </c>
       <c r="K30">
-        <v>67.36430851227671</v>
+        <v>121.9470370540949</v>
       </c>
       <c r="L30">
-        <v>10.05345834057636</v>
+        <v>8.407410844102706</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1456,25 +1456,25 @@
         <v>40</v>
       </c>
       <c r="C31">
-        <v>1453.400447957758</v>
+        <v>1453.401601517224</v>
       </c>
       <c r="D31">
-        <v>0.00509</v>
+        <v>0.00893</v>
       </c>
       <c r="E31">
-        <v>1122.824621868664</v>
+        <v>1122.824922708426</v>
       </c>
       <c r="G31">
-        <v>330.5758260890943</v>
+        <v>330.5766788087976</v>
       </c>
       <c r="H31">
-        <v>0.9997029665167717</v>
+        <v>0.9997003877915571</v>
       </c>
       <c r="K31">
-        <v>70.56699102047263</v>
+        <v>129.2738973053741</v>
       </c>
       <c r="L31">
-        <v>9.625953767898139</v>
+        <v>7.661650232243996</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1485,25 +1485,25 @@
         <v>41</v>
       </c>
       <c r="C32">
-        <v>1453.399341502143</v>
+        <v>1453.400543492322</v>
       </c>
       <c r="D32">
-        <v>0.0054</v>
+        <v>0.009090000000000001</v>
       </c>
       <c r="E32">
-        <v>1122.818404086196</v>
+        <v>1122.818903959232</v>
       </c>
       <c r="G32">
-        <v>330.5809374159478</v>
+        <v>330.5816395330899</v>
       </c>
       <c r="H32">
-        <v>0.9996875094590896</v>
+        <v>0.9996853862385197</v>
       </c>
       <c r="K32">
-        <v>74.06774739828927</v>
+        <v>129.694726144793</v>
       </c>
       <c r="L32">
-        <v>10.05868096167292</v>
+        <v>8.071521984273474</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1514,25 +1514,25 @@
         <v>42</v>
       </c>
       <c r="C33">
-        <v>1453.393353106094</v>
+        <v>1453.394462642341</v>
       </c>
       <c r="D33">
-        <v>0.00539</v>
+        <v>0.0091</v>
       </c>
       <c r="E33">
-        <v>1122.82209167855</v>
+        <v>1122.822525904418</v>
       </c>
       <c r="G33">
-        <v>330.571261427544</v>
+        <v>330.5719367379227</v>
       </c>
       <c r="H33">
-        <v>0.9997167708192792</v>
+        <v>0.9997147285433445</v>
       </c>
       <c r="K33">
-        <v>71.45448274948026</v>
+        <v>125.1177380391501</v>
       </c>
       <c r="L33">
-        <v>9.70045913112113</v>
+        <v>7.617374790551164</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1543,25 +1543,25 @@
         <v>43</v>
       </c>
       <c r="C34">
-        <v>1453.396642428989</v>
+        <v>1453.397780871216</v>
       </c>
       <c r="D34">
-        <v>0.00504</v>
+        <v>0.008789999999999999</v>
       </c>
       <c r="E34">
-        <v>1122.819355540085</v>
+        <v>1122.819869492535</v>
       </c>
       <c r="G34">
-        <v>330.5772868889042</v>
+        <v>330.5779113786807</v>
       </c>
       <c r="H34">
-        <v>0.9996985488935372</v>
+        <v>0.9996966603779954</v>
       </c>
       <c r="K34">
-        <v>69.37633575905318</v>
+        <v>126.7064014061152</v>
       </c>
       <c r="L34">
-        <v>9.971664607386288</v>
+        <v>7.979708799656366</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1572,25 +1572,25 @@
         <v>44</v>
       </c>
       <c r="C35">
-        <v>1453.42117406325</v>
+        <v>1453.422640182946</v>
       </c>
       <c r="D35">
-        <v>0.00546</v>
+        <v>0.0089</v>
       </c>
       <c r="E35">
-        <v>1122.846108597913</v>
+        <v>1122.846603897801</v>
       </c>
       <c r="G35">
-        <v>330.575065465337</v>
+        <v>330.5760362851454</v>
       </c>
       <c r="H35">
-        <v>0.9997052667441815</v>
+        <v>0.9997023308578227</v>
       </c>
       <c r="K35">
-        <v>82.79049457177886</v>
+        <v>142.5732648731567</v>
       </c>
       <c r="L35">
-        <v>10.38007526289315</v>
+        <v>8.3728684629017</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1601,25 +1601,25 @@
         <v>45</v>
       </c>
       <c r="C36">
-        <v>1453.391439211868</v>
+        <v>1453.392599265171</v>
       </c>
       <c r="D36">
-        <v>0.0056</v>
+        <v>0.009429999999999999</v>
       </c>
       <c r="E36">
-        <v>1122.813154078538</v>
+        <v>1122.813721229701</v>
       </c>
       <c r="G36">
-        <v>330.5782851333302</v>
+        <v>330.5788780354699</v>
       </c>
       <c r="H36">
-        <v>0.9996955301123619</v>
+        <v>0.999693737131448</v>
       </c>
       <c r="K36">
-        <v>78.0359040861448</v>
+        <v>137.7895734036047</v>
       </c>
       <c r="L36">
-        <v>10.01135315219194</v>
+        <v>7.643425769965168</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1630,25 +1630,25 @@
         <v>46</v>
       </c>
       <c r="C37">
-        <v>1453.380808976463</v>
+        <v>1453.381885144268</v>
       </c>
       <c r="D37">
-        <v>0.0055</v>
+        <v>0.00942</v>
       </c>
       <c r="E37">
-        <v>1122.814442000972</v>
+        <v>1122.814806923937</v>
       </c>
       <c r="G37">
-        <v>330.5663669754908</v>
+        <v>330.5670782203308</v>
       </c>
       <c r="H37">
-        <v>0.9997315728871552</v>
+        <v>0.9997294218746394</v>
       </c>
       <c r="K37">
-        <v>76.73204017723197</v>
+        <v>135.6687649481535</v>
       </c>
       <c r="L37">
-        <v>10.00019890140843</v>
+        <v>8.049321423815151</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1659,25 +1659,25 @@
         <v>47</v>
       </c>
       <c r="C38">
-        <v>1453.381877851455</v>
+        <v>1453.3829335648</v>
       </c>
       <c r="D38">
-        <v>0.00528</v>
+        <v>0.00911</v>
       </c>
       <c r="E38">
-        <v>1122.81014792934</v>
+        <v>1122.810632242587</v>
       </c>
       <c r="G38">
-        <v>330.5717299221151</v>
+        <v>330.5723013222132</v>
       </c>
       <c r="H38">
-        <v>0.999715353995524</v>
+        <v>0.9997136259697665</v>
       </c>
       <c r="K38">
-        <v>72.42450496876272</v>
+        <v>130.3190839764335</v>
       </c>
       <c r="L38">
-        <v>11.55881110395666</v>
+        <v>8.786418231503848</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1688,25 +1688,25 @@
         <v>48</v>
       </c>
       <c r="C39">
-        <v>1453.377736787716</v>
+        <v>1453.378793623494</v>
       </c>
       <c r="D39">
-        <v>0.00527</v>
+        <v>0.009039999999999999</v>
       </c>
       <c r="E39">
-        <v>1122.802765081988</v>
+        <v>1122.803140677137</v>
       </c>
       <c r="G39">
-        <v>330.5749717057274</v>
+        <v>330.5756529463572</v>
       </c>
       <c r="H39">
-        <v>0.9997055502864444</v>
+        <v>0.9997034901225074</v>
       </c>
       <c r="K39">
-        <v>70.82146508307555</v>
+        <v>127.2180474309758</v>
       </c>
       <c r="L39">
-        <v>10.91009441380701</v>
+        <v>9.015574923051826</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1717,25 +1717,25 @@
         <v>49</v>
       </c>
       <c r="C40">
-        <v>1453.383623333149</v>
+        <v>1453.384670318958</v>
       </c>
       <c r="D40">
-        <v>0.00509</v>
+        <v>0.008880000000000001</v>
       </c>
       <c r="E40">
-        <v>1122.809097891849</v>
+        <v>1122.80955534758</v>
       </c>
       <c r="G40">
-        <v>330.5745254413002</v>
+        <v>330.5751149713783</v>
       </c>
       <c r="H40">
-        <v>0.9997068998551208</v>
+        <v>0.9997051170310061</v>
       </c>
       <c r="K40">
-        <v>70.72534639751761</v>
+        <v>130.7415489534969</v>
       </c>
       <c r="L40">
-        <v>9.905022921558992</v>
+        <v>7.785550759839569</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1746,25 +1746,25 @@
         <v>50</v>
       </c>
       <c r="C41">
-        <v>1453.385768639576</v>
+        <v>1453.386903461384</v>
       </c>
       <c r="D41">
-        <v>0.00543</v>
+        <v>0.00927</v>
       </c>
       <c r="E41">
-        <v>1122.812503600261</v>
+        <v>1122.812864216747</v>
       </c>
       <c r="G41">
-        <v>330.5732650393152</v>
+        <v>330.5740392446371</v>
       </c>
       <c r="H41">
-        <v>0.9997107115141215</v>
+        <v>0.9997083701888467</v>
       </c>
       <c r="K41">
-        <v>75.29525449741024</v>
+        <v>135.0905793166658</v>
       </c>
       <c r="L41">
-        <v>9.744415955950508</v>
+        <v>7.832731676985745</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1775,25 +1775,25 @@
         <v>51</v>
       </c>
       <c r="C42">
-        <v>1453.386475023794</v>
+        <v>1453.38758362887</v>
       </c>
       <c r="D42">
-        <v>0.00572</v>
+        <v>0.009480000000000001</v>
       </c>
       <c r="E42">
-        <v>1122.809539976261</v>
+        <v>1122.809981699338</v>
       </c>
       <c r="G42">
-        <v>330.5769350475337</v>
+        <v>330.5776019295322</v>
       </c>
       <c r="H42">
-        <v>0.9996996128979193</v>
+        <v>0.9996975961802957</v>
       </c>
       <c r="K42">
-        <v>80.85785184040662</v>
+        <v>140.5558169091372</v>
       </c>
       <c r="L42">
-        <v>10.18666808806533</v>
+        <v>8.398479640185641</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -1804,25 +1804,25 @@
         <v>52</v>
       </c>
       <c r="C43">
-        <v>1453.393908954297</v>
+        <v>1453.395062947926</v>
       </c>
       <c r="D43">
-        <v>0.00514</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E43">
-        <v>1122.819318419906</v>
+        <v>1122.819839413621</v>
       </c>
       <c r="G43">
-        <v>330.5745905343908</v>
+        <v>330.5752235343052</v>
       </c>
       <c r="H43">
-        <v>0.9997067030038997</v>
+        <v>0.9997047887217262</v>
       </c>
       <c r="K43">
-        <v>70.61255737951812</v>
+        <v>130.3490042368046</v>
       </c>
       <c r="L43">
-        <v>9.42452838865912</v>
+        <v>7.544107405054101</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -1833,25 +1833,25 @@
         <v>53</v>
       </c>
       <c r="C44">
-        <v>1453.39077408753</v>
+        <v>1453.391926478266</v>
       </c>
       <c r="D44">
-        <v>0.00563</v>
+        <v>0.00937</v>
       </c>
       <c r="E44">
-        <v>1122.826318059849</v>
+        <v>1122.826842595969</v>
       </c>
       <c r="G44">
-        <v>330.5644560276808</v>
+        <v>330.5650838822962</v>
       </c>
       <c r="H44">
-        <v>0.9997373521983457</v>
+        <v>0.9997354533598372</v>
       </c>
       <c r="K44">
-        <v>77.73968095683399</v>
+        <v>134.7144352748837</v>
       </c>
       <c r="L44">
-        <v>10.10721584394441</v>
+        <v>7.973751296550429</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -1862,25 +1862,25 @@
         <v>54</v>
       </c>
       <c r="C45">
-        <v>1453.396636697844</v>
+        <v>1453.397775464695</v>
       </c>
       <c r="D45">
-        <v>0.00525</v>
+        <v>0.00902</v>
       </c>
       <c r="E45">
-        <v>1122.826928023729</v>
+        <v>1122.827574547163</v>
       </c>
       <c r="G45">
-        <v>330.5697086741147</v>
+        <v>330.5702009175322</v>
       </c>
       <c r="H45">
-        <v>0.9997214666931099</v>
+        <v>0.9997199780340899</v>
       </c>
       <c r="K45">
-        <v>73.0407735221128</v>
+        <v>131.2139878072483</v>
       </c>
       <c r="L45">
-        <v>9.103623558200121</v>
+        <v>6.791356523447781</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -1891,25 +1891,25 @@
         <v>55</v>
       </c>
       <c r="C46">
-        <v>1453.413334456106</v>
+        <v>1453.414767089628</v>
       </c>
       <c r="D46">
-        <v>0.00557</v>
+        <v>0.00902</v>
       </c>
       <c r="E46">
-        <v>1122.847538036607</v>
+        <v>1122.848071599876</v>
       </c>
       <c r="G46">
-        <v>330.5657964194991</v>
+        <v>330.5666954897526</v>
       </c>
       <c r="H46">
-        <v>0.9997332984221176</v>
+        <v>0.9997305793627496</v>
       </c>
       <c r="K46">
-        <v>85.18130582244868</v>
+        <v>143.0739984750954</v>
       </c>
       <c r="L46">
-        <v>9.598963172327906</v>
+        <v>7.81241414741933</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -1920,25 +1920,25 @@
         <v>56</v>
       </c>
       <c r="C47">
-        <v>1453.397741641965</v>
+        <v>1453.060478930247</v>
       </c>
       <c r="D47">
-        <v>0.00508</v>
+        <v>0.0718</v>
       </c>
       <c r="E47">
-        <v>1122.820992948766</v>
+        <v>1122.821642936284</v>
       </c>
       <c r="G47">
-        <v>330.5767486931986</v>
+        <v>330.2388359939628</v>
       </c>
       <c r="H47">
-        <v>0.9997001764534548</v>
+        <v>1.000723106975951</v>
       </c>
       <c r="K47">
-        <v>71.26410326433248</v>
+        <v>565.5378728571397</v>
       </c>
       <c r="L47">
-        <v>10.58991231802186</v>
+        <v>8.348503647701705</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -1949,25 +1949,25 @@
         <v>57</v>
       </c>
       <c r="C48">
-        <v>1453.407611750721</v>
+        <v>1453.408901871221</v>
       </c>
       <c r="D48">
-        <v>0.00541</v>
+        <v>0.009090000000000001</v>
       </c>
       <c r="E48">
-        <v>1122.849948064746</v>
+        <v>1122.850504082111</v>
       </c>
       <c r="G48">
-        <v>330.5576636859751</v>
+        <v>330.5583977891108</v>
       </c>
       <c r="H48">
-        <v>0.9997578949310004</v>
+        <v>0.9997556746715528</v>
       </c>
       <c r="K48">
-        <v>76.9638406893331</v>
+        <v>135.2066642500835</v>
       </c>
       <c r="L48">
-        <v>9.444470338350595</v>
+        <v>7.297016497033685</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -1978,25 +1978,25 @@
         <v>58</v>
       </c>
       <c r="C49">
-        <v>1453.405414463208</v>
+        <v>1453.406691796038</v>
       </c>
       <c r="D49">
-        <v>0.00519</v>
+        <v>0.008829999999999999</v>
       </c>
       <c r="E49">
-        <v>1122.83580597472</v>
+        <v>1122.836409143468</v>
       </c>
       <c r="G49">
-        <v>330.5696084884878</v>
+        <v>330.5702826525694</v>
       </c>
       <c r="H49">
-        <v>0.9997217696783793</v>
+        <v>0.9997197308486838</v>
       </c>
       <c r="K49">
-        <v>76.11046656623463</v>
+        <v>133.7801774046319</v>
       </c>
       <c r="L49">
-        <v>9.379609420641051</v>
+        <v>7.185977440536771</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2007,25 +2007,25 @@
         <v>59</v>
       </c>
       <c r="C50">
-        <v>1453.405556310761</v>
+        <v>1453.406832589812</v>
       </c>
       <c r="D50">
-        <v>0.00524</v>
+        <v>0.00891</v>
       </c>
       <c r="E50">
-        <v>1122.844390478282</v>
+        <v>1122.84487525295</v>
       </c>
       <c r="G50">
-        <v>330.5611658324785</v>
+        <v>330.561957336862</v>
       </c>
       <c r="H50">
-        <v>0.9997473029468898</v>
+        <v>0.9997449091312828</v>
       </c>
       <c r="K50">
-        <v>76.14211553110935</v>
+        <v>135.6514483380049</v>
       </c>
       <c r="L50">
-        <v>9.726788815239493</v>
+        <v>8.170984803226464</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2036,25 +2036,25 @@
         <v>60</v>
       </c>
       <c r="C51">
-        <v>1453.405442589789</v>
+        <v>1453.406758886178</v>
       </c>
       <c r="D51">
-        <v>0.00509</v>
+        <v>0.008710000000000001</v>
       </c>
       <c r="E51">
-        <v>1122.84505842183</v>
+        <v>1122.84558410428</v>
       </c>
       <c r="G51">
-        <v>330.5603841679592</v>
+        <v>330.561174781898</v>
       </c>
       <c r="H51">
-        <v>0.9997496670141902</v>
+        <v>0.9997472758803175</v>
       </c>
       <c r="K51">
-        <v>72.25880885877866</v>
+        <v>130.9274736238403</v>
       </c>
       <c r="L51">
-        <v>9.762773122800894</v>
+        <v>7.706331466658581</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2065,25 +2065,25 @@
         <v>61</v>
       </c>
       <c r="C52">
-        <v>1453.419250753629</v>
+        <v>1453.420683717182</v>
       </c>
       <c r="D52">
-        <v>0.0057</v>
+        <v>0.00911</v>
       </c>
       <c r="E52">
-        <v>1122.849118101238</v>
+        <v>1122.849571161952</v>
       </c>
       <c r="G52">
-        <v>330.5701326523906</v>
+        <v>330.5711125552295</v>
       </c>
       <c r="H52">
-        <v>0.9997201844835515</v>
+        <v>0.9997172210405593</v>
       </c>
       <c r="K52">
-        <v>74.88954204787636</v>
+        <v>126.786946133707</v>
       </c>
       <c r="L52">
-        <v>9.822855860583395</v>
+        <v>8.693326811091882</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2094,25 +2094,25 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>1453.415035925438</v>
+        <v>1453.415948616025</v>
       </c>
       <c r="D53">
-        <v>0.012</v>
+        <v>0.0124</v>
       </c>
       <c r="E53">
-        <v>1122.839618165037</v>
+        <v>1122.840162683653</v>
       </c>
       <c r="G53">
-        <v>330.5754177604013</v>
+        <v>330.5757859323712</v>
       </c>
       <c r="H53">
-        <v>0.9997042013557339</v>
+        <v>0.9997030879557789</v>
       </c>
       <c r="K53">
-        <v>122.4226010566517</v>
+        <v>174.8591000185636</v>
       </c>
       <c r="L53">
-        <v>10.81618114290306</v>
+        <v>8.695043255343741</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2123,25 +2123,25 @@
         <v>63</v>
       </c>
       <c r="C54">
-        <v>1453.406451519354</v>
+        <v>1453.407788070906</v>
       </c>
       <c r="D54">
-        <v>0.00536</v>
+        <v>0.008869999999999999</v>
       </c>
       <c r="E54">
-        <v>1122.840892087685</v>
+        <v>1122.84130747438</v>
       </c>
       <c r="G54">
-        <v>330.565559431669</v>
+        <v>330.5664805965268</v>
       </c>
       <c r="H54">
-        <v>0.9997340151471914</v>
+        <v>0.9997312292632741</v>
       </c>
       <c r="K54">
-        <v>79.79347161703726</v>
+        <v>137.1657955058886</v>
       </c>
       <c r="L54">
-        <v>9.313980223547709</v>
+        <v>7.541847754085374</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -2152,25 +2152,25 @@
         <v>64</v>
       </c>
       <c r="C55">
-        <v>1453.407824808408</v>
+        <v>1453.409192798567</v>
       </c>
       <c r="D55">
-        <v>0.00569</v>
+        <v>0.00932</v>
       </c>
       <c r="E55">
-        <v>1122.833860502961</v>
+        <v>1122.834464511721</v>
       </c>
       <c r="G55">
-        <v>330.5739643054467</v>
+        <v>330.5747282868465</v>
       </c>
       <c r="H55">
-        <v>0.9997085968169058</v>
+        <v>0.99970628642017</v>
       </c>
       <c r="K55">
-        <v>82.40410650638815</v>
+        <v>141.5988414094012</v>
       </c>
       <c r="L55">
-        <v>10.58547432059827</v>
+        <v>7.48395639693156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>